<commit_message>
updated values for order sheet
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70A9CA0-3C65-4E1F-A5C7-932CEF668B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1120" yWindow="450" windowWidth="16510" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="clients" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="vendors" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Kates Car and Co." sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Owens Cafe" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="SA-Technology" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Client Database" sheetId="6" r:id="rId9"/>
+    <sheet name="clients" sheetId="1" r:id="rId1"/>
+    <sheet name="vendors" sheetId="2" r:id="rId2"/>
+    <sheet name="Kates Car and Co." sheetId="3" r:id="rId3"/>
+    <sheet name="Owens Cafe" sheetId="4" r:id="rId4"/>
+    <sheet name="SA-Technology" sheetId="5" r:id="rId5"/>
+    <sheet name="Client Database" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -54,9 +63,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Order:</t>
-  </si>
-  <si>
     <t>Tires</t>
   </si>
   <si>
@@ -118,37 +124,61 @@
   </si>
   <si>
     <t>Items Not Found</t>
+  </si>
+  <si>
+    <t>Order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,87 +186,56 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -426,32 +425,37 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.29"/>
-    <col customWidth="1" min="2" max="2" width="22.71"/>
-    <col customWidth="1" min="3" max="3" width="21.57"/>
-    <col customWidth="1" min="4" max="4" width="25.57"/>
-    <col customWidth="1" min="5" max="5" width="17.86"/>
-    <col customWidth="1" min="6" max="6" width="26.86"/>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -467,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -483,139 +487,160 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="7" t="s">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="7" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>16</v>
+      <c r="E7">
+        <v>2</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.0"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -640,23 +665,23 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="9">
         <v>24.99</v>
       </c>
       <c r="C2" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9">
         <v>4.99</v>
@@ -665,12 +690,12 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="7">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9">
         <v>12.99</v>
@@ -679,36 +704,37 @@
         <v>0.1</v>
       </c>
       <c r="D4" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -733,9 +759,9 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="10">
         <v>2.99</v>
@@ -744,64 +770,65 @@
         <v>0.1</v>
       </c>
       <c r="D2" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="9">
         <v>1.99</v>
       </c>
       <c r="C3" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>0.5</v>
       </c>
       <c r="D4" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -826,69 +853,70 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="12">
-        <v>1999.0</v>
+        <v>1999</v>
       </c>
       <c r="C2" s="7">
         <v>0.1</v>
       </c>
       <c r="D2" s="7">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="12">
-        <v>2999.0</v>
+        <v>2999</v>
       </c>
       <c r="C3" s="7">
         <v>0.5</v>
       </c>
       <c r="D3" s="7">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="9">
         <v>14.99</v>
       </c>
       <c r="C4" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="4" width="15.0"/>
-    <col customWidth="1" min="6" max="6" width="18.0"/>
-    <col customWidth="1" min="7" max="7" width="16.43"/>
+    <col min="3" max="4" width="15" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -899,16 +927,16 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -934,6 +962,6 @@
       <c r="AC1" s="8"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
gitignore and start of first do while loop for vendor add
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70A9CA0-3C65-4E1F-A5C7-932CEF668B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB383DE-503E-4A0E-92C6-3AAFF30137E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="450" windowWidth="16510" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -437,8 +437,8 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -451,11 +451,11 @@
     <col min="6" max="6" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -586,14 +586,16 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +631,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -723,7 +725,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -817,7 +819,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -907,7 +909,7 @@
   </sheetPr>
   <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
add function is working
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB383DE-503E-4A0E-92C6-3AAFF30137E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2B68B5-4A67-434A-B1FD-221BBE6BD8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -81,10 +81,6 @@
     <t>Desktop</t>
   </si>
   <si>
-    <t xml:space="preserve">Kate's Car and Co.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Owen's Cafe
 </t>
   </si>
@@ -127,6 +123,12 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>Kates Car and Co.</t>
+  </si>
+  <si>
+    <t>test vendor</t>
   </si>
 </sst>
 </file>
@@ -512,7 +514,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>10</v>
@@ -584,10 +586,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -595,24 +597,29 @@
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="5" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -627,22 +634,24 @@
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -683,7 +692,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9">
         <v>4.99</v>
@@ -697,7 +706,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9">
         <v>12.99</v>
@@ -727,16 +736,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -791,7 +800,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -821,16 +830,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -929,16 +938,16 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>

</xml_diff>

<commit_message>
remove functionality test working
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD633603-2AB4-4A6D-A2B9-BC50A962DCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EE7F0D-8999-439F-BFBE-3DD8FED7BEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="3790" windowWidth="10320" windowHeight="7700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1510" yWindow="1640" windowWidth="13810" windowHeight="7700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -81,14 +81,6 @@
     <t>Desktop</t>
   </si>
   <si>
-    <t xml:space="preserve">Owen's Cafe
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA-Technology
-</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -126,6 +118,15 @@
   </si>
   <si>
     <t>Kates Car and Co.</t>
+  </si>
+  <si>
+    <t>Owen's Café</t>
+  </si>
+  <si>
+    <t>SA Technology</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
   <si>
     <t>Test vendor</t>
@@ -208,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -225,6 +226,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,7 +527,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>10</v>
@@ -592,10 +599,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -604,31 +611,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>31</v>
+      <c r="A2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+    </row>
+    <row r="7" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -650,16 +663,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -700,7 +713,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="9">
         <v>4.99</v>
@@ -714,7 +727,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="9">
         <v>12.99</v>
@@ -744,16 +757,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -808,7 +821,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -838,16 +851,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -946,16 +959,16 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>

</xml_diff>

<commit_message>
updated remove option with confirmation message box
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EE7F0D-8999-439F-BFBE-3DD8FED7BEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE40432-9F3B-4FC0-9962-613D9FFE8B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1510" yWindow="1640" windowWidth="13810" windowHeight="7700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>Test vendor</t>
   </si>
 </sst>
 </file>
@@ -617,23 +614,21 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>30</v>
-      </c>
+      <c r="A5" s="16"/>
     </row>
     <row r="6" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>

</xml_diff>

<commit_message>
rename BruteForceAddVendor to AddVendor and start of AddClient
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE40432-9F3B-4FC0-9962-613D9FFE8B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8B5010-33B5-4818-BB72-5C5FAEECA249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -596,7 +596,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -623,20 +623,23 @@
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-    </row>
-    <row r="6" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-    </row>
-    <row r="7" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-    </row>
-    <row r="8" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+    </row>
+    <row r="8" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+    </row>
+    <row r="9" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
hardcode AddClient for single client - one client only
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB6B778-64AE-437B-94B8-AB9435A3082C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB4775D-15E4-4871-84A7-39EB68AD22D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="890" windowWidth="16700" windowHeight="8110" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17565" yWindow="2745" windowWidth="14175" windowHeight="12135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="clients" sheetId="1" r:id="rId1"/>
-    <sheet name="vendors" sheetId="2" r:id="rId2"/>
-    <sheet name="Kates Car and Co." sheetId="3" r:id="rId3"/>
-    <sheet name="Owens Cafe" sheetId="4" r:id="rId4"/>
-    <sheet name="SA-Technology" sheetId="5" r:id="rId5"/>
-    <sheet name="Client Database" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
+    <sheet name="clients" sheetId="1" r:id="rId2"/>
+    <sheet name="vendors" sheetId="2" r:id="rId3"/>
+    <sheet name="Kates Car and Co." sheetId="3" r:id="rId4"/>
+    <sheet name="Owens Cafe" sheetId="4" r:id="rId5"/>
+    <sheet name="SA-Technology" sheetId="5" r:id="rId6"/>
+    <sheet name="Client Database" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -137,7 +138,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -185,6 +186,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -229,6 +237,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,14 +452,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -463,11 +486,11 @@
     <col min="6" max="6" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -483,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -499,7 +522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -521,8 +544,20 @@
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>27</v>
       </c>
@@ -545,7 +580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
@@ -565,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -591,14 +626,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -627,26 +662,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-    </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-    </row>
-    <row r="9" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A8" s="15"/>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-    </row>
-    <row r="11" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
+      <c r="A10" s="17"/>
+    </row>
+    <row r="11" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -742,7 +777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -836,7 +871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -930,7 +965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
renamed xamls, structured excel client sheet, and addclient_structured
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB4775D-15E4-4871-84A7-39EB68AD22D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE42BDC5-135B-497D-BDEB-30FC012D0889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17565" yWindow="2745" windowWidth="14175" windowHeight="12135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
-    <sheet name="clients" sheetId="1" r:id="rId2"/>
+    <sheet name="clients" sheetId="1" r:id="rId1"/>
+    <sheet name="clients_structured" sheetId="7" r:id="rId2"/>
     <sheet name="vendors" sheetId="2" r:id="rId3"/>
     <sheet name="Kates Car and Co." sheetId="3" r:id="rId4"/>
     <sheet name="Owens Cafe" sheetId="4" r:id="rId5"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>Order No.</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,25 +151,30 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -183,6 +191,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -214,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -238,6 +252,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,28 +473,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -486,11 +493,11 @@
     <col min="6" max="6" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -506,7 +513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -522,7 +529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -544,20 +551,8 @@
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>27</v>
       </c>
@@ -580,7 +575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
@@ -600,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -623,6 +618,205 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="19" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>1</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="18">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="38" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>2</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>2</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>3</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>3</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
addclient: remove by client order number and remove by client name
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE42BDC5-135B-497D-BDEB-30FC012D0889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6398662-2334-4B3A-9CC8-9A028D9AEA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>Order No.</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -623,10 +629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -653,6 +659,12 @@
       <c r="E1" s="19" t="s">
         <v>9</v>
       </c>
+      <c r="F1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="18">
@@ -814,6 +826,9 @@
       <c r="E10">
         <v>3</v>
       </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
search for addclient added and two test customers in excel sheet
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6398662-2334-4B3A-9CC8-9A028D9AEA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8704781B-1904-4726-8463-0B4B34512064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>testcustomer1</t>
+  </si>
+  <si>
+    <t>testcustomer2</t>
+  </si>
+  <si>
+    <t>testcustomer1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -629,10 +638,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -828,7 +837,38 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added inventory sheet and renamed client database sheet to expense_reports
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8704781B-1904-4726-8463-0B4B34512064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D55FE8F-24D0-4C24-BA46-78714D1B91DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24630" yWindow="3795" windowWidth="23415" windowHeight="10410" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
     <sheet name="clients_structured" sheetId="7" r:id="rId2"/>
     <sheet name="vendors" sheetId="2" r:id="rId3"/>
-    <sheet name="Kates Car and Co." sheetId="3" r:id="rId4"/>
-    <sheet name="Owens Cafe" sheetId="4" r:id="rId5"/>
-    <sheet name="SA-Technology" sheetId="5" r:id="rId6"/>
-    <sheet name="Client Database" sheetId="6" r:id="rId7"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId4"/>
+    <sheet name="inventory" sheetId="8" r:id="rId5"/>
+    <sheet name="Kates Car and Co." sheetId="3" r:id="rId6"/>
+    <sheet name="Owens Cafe" sheetId="4" r:id="rId7"/>
+    <sheet name="SA-Technology" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -255,7 +256,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -274,6 +274,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +546,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="6">
@@ -568,7 +569,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -640,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -652,107 +653,107 @@
     <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="19" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:7" s="18" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
-        <v>1</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="A3" s="17">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
-        <v>1</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
-        <v>2</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="A5" s="17">
+        <v>2</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>1</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="38" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
-        <v>2</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="A6" s="17">
+        <v>2</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -765,13 +766,13 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
-        <v>2</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="A7" s="17">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -784,13 +785,13 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="17">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -802,13 +803,13 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="17">
         <v>3</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -823,10 +824,10 @@
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -840,10 +841,10 @@
       <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -857,10 +858,10 @@
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -912,13 +913,13 @@
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
     </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
     </row>
     <row r="10" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+      <c r="A10" s="16"/>
     </row>
     <row r="11" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -931,6 +932,88 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:AC1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="15" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -938,7 +1021,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1026,14 +1109,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1080,7 +1165,7 @@
       <c r="B2" s="10">
         <v>2.99</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="21">
         <v>0.1</v>
       </c>
       <c r="D2" s="2">
@@ -1117,10 +1202,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1171,7 +1257,7 @@
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>1999</v>
       </c>
       <c r="C2" s="7">
@@ -1185,7 +1271,7 @@
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>2999</v>
       </c>
       <c r="C3" s="7">
@@ -1208,72 +1294,6 @@
       <c r="D4" s="7">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:AC1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="4" width="15" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bugfix for search in AddVendor
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D248386-DBC0-4B62-91D0-AE6317DCE1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD7C4CB-CEDC-458E-B849-F462B315601A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24210" yWindow="4560" windowWidth="23415" windowHeight="10410" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23685" yWindow="5070" windowWidth="23415" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -138,15 +138,6 @@
   </si>
   <si>
     <t>Column2</t>
-  </si>
-  <si>
-    <t>testcustomer1</t>
-  </si>
-  <si>
-    <t>testcustomer2</t>
-  </si>
-  <si>
-    <t>testcustomer1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -635,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -832,38 +823,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -875,10 +842,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -906,19 +873,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-    </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-    </row>
-    <row r="10" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A9" s="11"/>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
     </row>
     <row r="11" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-    </row>
-    <row r="12" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
+      <c r="A11" s="13"/>
+    </row>
+    <row r="12" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="13" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1207,8 +1174,8 @@
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DiscountTest working for one vendor
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD7C4CB-CEDC-458E-B849-F462B315601A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992B7307-CD93-435C-A67F-C62B6F002882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23685" yWindow="5070" windowWidth="23415" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26085" yWindow="1275" windowWidth="16545" windowHeight="12900" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -981,11 +981,14 @@
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Items are now taking from the vendor list and we are pulling from them to make a table and adding it to inventory. Need to add recursion.
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70A9CA0-3C65-4E1F-A5C7-932CEF668B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F154D-0B98-4733-8249-17E55ABE58C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="450" windowWidth="16510" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25425" yWindow="1035" windowWidth="24105" windowHeight="16515" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
     <sheet name="vendors" sheetId="2" r:id="rId2"/>
     <sheet name="Kates Car and Co." sheetId="3" r:id="rId3"/>
-    <sheet name="Owens Cafe" sheetId="4" r:id="rId4"/>
-    <sheet name="SA-Technology" sheetId="5" r:id="rId5"/>
-    <sheet name="Client Database" sheetId="6" r:id="rId6"/>
+    <sheet name="Inventory" sheetId="7" r:id="rId4"/>
+    <sheet name="Owens Cafe" sheetId="4" r:id="rId5"/>
+    <sheet name="SA-Technology" sheetId="5" r:id="rId6"/>
+    <sheet name="Client Database" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -81,10 +82,6 @@
     <t>Desktop</t>
   </si>
   <si>
-    <t xml:space="preserve">Kate's Car and Co.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Owen's Cafe
 </t>
   </si>
@@ -127,6 +124,10 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kates Car and Co.
+</t>
   </si>
 </sst>
 </file>
@@ -201,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -217,6 +218,9 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,25 +441,25 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -471,7 +475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -487,7 +491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -510,9 +514,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>10</v>
@@ -533,7 +537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
@@ -553,7 +557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -586,31 +590,31 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -625,22 +629,24 @@
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -665,7 +671,7 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -679,9 +685,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9">
         <v>4.99</v>
@@ -693,9 +699,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9">
         <v>12.99</v>
@@ -708,33 +714,50 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0723A4-D515-4CFA-B98E-6F07DE382EF4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -759,7 +782,7 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -773,7 +796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
@@ -787,9 +810,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
@@ -806,7 +829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -815,20 +838,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -853,7 +876,7 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -867,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -881,7 +904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
@@ -900,7 +923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -909,14 +932,14 @@
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -927,16 +950,16 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>

</xml_diff>

<commit_message>
rename clients_Structured to clients, inventory to vendor_inventory
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD04DA43-9554-46A1-BA6F-16DD36FC1C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9158F220-A9E5-455A-8A05-6C1010C354BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="610" windowWidth="15750" windowHeight="8890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21270" yWindow="1830" windowWidth="15750" windowHeight="8895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="clients_structured" sheetId="7" r:id="rId1"/>
+    <sheet name="clients" sheetId="7" r:id="rId1"/>
     <sheet name="vendors" sheetId="2" r:id="rId2"/>
-    <sheet name="inventory" sheetId="8" r:id="rId3"/>
+    <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
     <sheet name="expense_reports" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -455,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -719,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
P0 source datasheet updated with out_of_stock sheet, moved out of expense_reports
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9158F220-A9E5-455A-8A05-6C1010C354BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2113BD54-7C52-4431-8250-49EC90A5C218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21270" yWindow="1830" windowWidth="15750" windowHeight="8895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="770" windowWidth="15750" windowHeight="8900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
     <sheet name="vendors" sheetId="2" r:id="rId2"/>
     <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
     <sheet name="expense_reports" sheetId="6" r:id="rId4"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -455,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -717,15 +718,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
@@ -897,6 +900,9 @@
       <c r="E10" s="4">
         <v>1</v>
       </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -911,7 +917,7 @@
   <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -937,12 +943,8 @@
       <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -969,4 +971,34 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add vendor updated to use excel application scope for remove vendor option
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6E18BB-1A4E-44DB-9371-22C6FEFC9D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81F33F2-6352-4325-B9BE-D3FFFB8F4235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18735" yWindow="4560" windowWidth="15750" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18735" yWindow="4560" windowWidth="15750" windowHeight="8895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -462,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -678,9 +678,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -694,8 +694,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -709,19 +709,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-    </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-    </row>
-    <row r="11" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
     </row>
     <row r="12" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
renamed totalexpense to yu_testsequence
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81F33F2-6352-4325-B9BE-D3FFFB8F4235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A76571-9A08-461C-AE3F-71A87DF4451A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18735" yWindow="4560" windowWidth="15750" windowHeight="8895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18570" yWindow="465" windowWidth="18120" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -135,12 +135,6 @@
   </si>
   <si>
     <t>Vendor</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -221,11 +215,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -462,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -474,184 +467,172 @@
     <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="F1"/>
+      <c r="G1"/>
     </row>
     <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>1</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3"/>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="9">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="38" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
-        <v>2</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>2</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>3</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>3</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4"/>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E10">
@@ -659,14 +640,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -680,7 +661,7 @@
   </sheetPr>
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -690,12 +671,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -710,16 +691,16 @@
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7"/>
     </row>
     <row r="13" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -744,7 +725,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -764,16 +745,16 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <v>24.99</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>2</v>
       </c>
     </row>
@@ -781,16 +762,16 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>4.99</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0.5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>3</v>
       </c>
     </row>
@@ -798,30 +779,30 @@
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>12.99</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0.1</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>2.99</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.1</v>
       </c>
       <c r="E5" s="2">
@@ -829,13 +810,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>1.99</v>
       </c>
       <c r="D6" s="2">
@@ -846,75 +827,75 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>1</v>
       </c>
       <c r="D7" s="2">
         <v>0.5</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>1999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.1</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>2999</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.5</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>14.99</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -957,28 +938,28 @@
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1000,7 +981,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>

<commit_message>
Vendor Addition and Client Orders are collect, Need to run expense now.
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A76571-9A08-461C-AE3F-71A87DF4451A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477369C6-EDFB-4D52-BA98-A6A267DBE1F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18570" yWindow="465" windowWidth="18120" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
     <sheet name="vendors" sheetId="2" r:id="rId2"/>
     <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId4"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId5"/>
+    <sheet name="Hell" sheetId="11" r:id="rId4"/>
+    <sheet name="Test" sheetId="10" r:id="rId5"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -135,6 +137,21 @@
   </si>
   <si>
     <t>Vendor</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Hell</t>
+  </si>
+  <si>
+    <t>Souls</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -456,18 +473,18 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
@@ -483,10 +500,14 @@
       <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1"/>
-      <c r="G1"/>
-    </row>
-    <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -503,7 +524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -520,7 +541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -537,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -554,7 +575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -571,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -588,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -605,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>3</v>
       </c>
@@ -622,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -639,12 +660,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
@@ -659,50 +680,62 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-    </row>
-    <row r="13" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:1" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -714,17 +747,17 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
@@ -741,7 +774,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -755,10 +788,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -772,10 +805,10 @@
         <v>0.5</v>
       </c>
       <c r="E3" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -792,7 +825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
@@ -809,7 +842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
@@ -826,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
@@ -843,7 +876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
@@ -860,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
@@ -877,7 +910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
@@ -894,7 +927,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>5.99</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>6.99</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
     </row>
   </sheetData>
@@ -903,6 +970,158 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBA6BF3-9357-4785-B233-4123450A0704}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="13">
+        <v>6.99</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="13">
+        <v>5.99</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -913,14 +1132,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -966,7 +1185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -974,13 +1193,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Revert "P0 source datasheet updated with out_of_stock sheet, moved out of expense_reports"
This reverts commit 07aebe3fdd64633332e3df83958243b18dfc1425.
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,23 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2113BD54-7C52-4431-8250-49EC90A5C218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9158F220-A9E5-455A-8A05-6C1010C354BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="770" windowWidth="15750" windowHeight="8900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21270" yWindow="1830" windowWidth="15750" windowHeight="8895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
     <sheet name="vendors" sheetId="2" r:id="rId2"/>
     <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
     <sheet name="expense_reports" sheetId="6" r:id="rId4"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -456,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -718,17 +717,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
@@ -900,9 +897,6 @@
       <c r="E10" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -917,7 +911,7 @@
   <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -943,8 +937,12 @@
       <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -971,34 +969,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
It takes a name and and and order and gives a price
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477369C6-EDFB-4D52-BA98-A6A267DBE1F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074DD67-CA29-4D95-A7F4-F9F2150EFF92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -521,7 +521,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -538,7 +538,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
rough recorded macro for shipment update
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,32 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074DD67-CA29-4D95-A7F4-F9F2150EFF92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40A4814-D71A-4F26-A69F-D609BD63B491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2310" yWindow="1500" windowWidth="15330" windowHeight="8290" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
-    <sheet name="vendors" sheetId="2" r:id="rId2"/>
-    <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
-    <sheet name="Hell" sheetId="11" r:id="rId4"/>
-    <sheet name="Test" sheetId="10" r:id="rId5"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="13" r:id="rId3"/>
+    <sheet name="vendors" sheetId="2" r:id="rId4"/>
+    <sheet name="vendor_inventory" sheetId="8" r:id="rId5"/>
+    <sheet name="Hell" sheetId="11" r:id="rId6"/>
+    <sheet name="Test" sheetId="10" r:id="rId7"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId8"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +154,12 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>Dark Souls</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -472,19 +480,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
@@ -507,7 +515,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -524,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -541,7 +549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -558,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -575,7 +583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -592,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -609,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -626,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>3</v>
       </c>
@@ -643,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -660,12 +668,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
@@ -676,6 +684,502 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F942F23-3EB7-4CF5-8038-49C58384291D}">
+  <dimension ref="A12:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C32DEE9-1E27-4894-A3AA-A373D548A27C}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate leftLabels="1" topLabels="1">
+    <dataRefs count="2">
+      <dataRef ref="B1" sheet="Sheet2"/>
+      <dataRef ref="B1:C1048576" sheet="Sheet2"/>
+    </dataRefs>
+  </dataConsolidate>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -686,78 +1190,77 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
@@ -770,11 +1273,12 @@
       <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -787,11 +1291,12 @@
       <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -804,11 +1309,12 @@
       <c r="D3" s="3">
         <v>0.5</v>
       </c>
-      <c r="E3" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -821,11 +1327,11 @@
       <c r="D4" s="3">
         <v>0.1</v>
       </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
@@ -838,11 +1344,11 @@
       <c r="D5" s="12">
         <v>0.1</v>
       </c>
-      <c r="E5" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
@@ -855,11 +1361,11 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
@@ -872,11 +1378,11 @@
       <c r="D7" s="2">
         <v>0.5</v>
       </c>
-      <c r="E7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
@@ -889,11 +1395,11 @@
       <c r="D8" s="3">
         <v>0.1</v>
       </c>
-      <c r="E8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
@@ -906,11 +1412,11 @@
       <c r="D9" s="3">
         <v>0.5</v>
       </c>
-      <c r="E9" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
@@ -923,11 +1429,11 @@
       <c r="D10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -941,11 +1447,11 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B12" t="s">
@@ -958,10 +1464,27 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>6.99</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
     </row>
   </sheetData>
@@ -969,7 +1492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBA6BF3-9357-4785-B233-4123450A0704}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -977,9 +1500,9 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
@@ -996,7 +1519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1018,7 +1541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1026,9 +1549,9 @@
       <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
@@ -1045,7 +1568,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1062,54 +1585,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="13"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="13"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="3"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="3"/>
       <c r="C6" s="13"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="3"/>
       <c r="C7" s="13"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="3"/>
       <c r="C8" s="13"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="3"/>
       <c r="C9" s="13"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="3"/>
       <c r="C10" s="13"/>
@@ -1121,7 +1644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1132,14 +1655,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1185,7 +1708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -1193,13 +1716,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
added choose person, next to add quantity control and discounts
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074DD67-CA29-4D95-A7F4-F9F2150EFF92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B08B5A-8BE0-4F82-AB12-DC93D25E06C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="1935" windowWidth="28800" windowHeight="15435" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Total Expenses</t>
   </si>
   <si>
-    <t>Total Items</t>
-  </si>
-  <si>
     <t>Items Out of Stock</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>SA Technology</t>
   </si>
   <si>
-    <t>Order No.</t>
-  </si>
-  <si>
     <t>Owens Café</t>
   </si>
   <si>
@@ -152,6 +146,12 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>Carson Goble</t>
+  </si>
+  <si>
+    <t>kcbku98@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -247,14 +247,35 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -486,7 +507,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -495,168 +516,168 @@
         <v>4</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8">
-        <v>1</v>
+      <c r="E2" s="15">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="A4" s="15">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="15">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+      <c r="A6" s="15">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="15">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+      <c r="A8" s="15">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+      <c r="A9" s="15">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="13">
         <v>3</v>
       </c>
     </row>
@@ -698,27 +719,27 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -747,7 +768,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -759,7 +780,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -776,29 +797,29 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="11">
         <v>24.99</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
       </c>
       <c r="E2" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <v>4.99</v>
       </c>
       <c r="D3" s="3">
@@ -810,12 +831,12 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>12.99</v>
       </c>
       <c r="D4" s="3">
@@ -827,15 +848,15 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>2.99</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>0.1</v>
       </c>
       <c r="E5" s="2">
@@ -844,29 +865,29 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>1.99</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <v>1</v>
       </c>
       <c r="D7" s="2">
@@ -878,12 +899,12 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="11">
         <v>1999</v>
       </c>
       <c r="D8" s="3">
@@ -895,12 +916,12 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>2999</v>
       </c>
       <c r="D9" s="3">
@@ -912,12 +933,12 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>14.99</v>
       </c>
       <c r="D10" s="3">
@@ -929,10 +950,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>5.99</v>
@@ -946,10 +967,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>6.99</v>
@@ -981,7 +1002,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -998,12 +1019,12 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="13">
+        <v>35</v>
+      </c>
+      <c r="C2" s="11">
         <v>6.99</v>
       </c>
       <c r="D2" s="3">
@@ -1030,7 +1051,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -1047,12 +1068,12 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="13">
+        <v>33</v>
+      </c>
+      <c r="C2" s="11">
         <v>5.99</v>
       </c>
       <c r="D2" s="3">
@@ -1064,55 +1085,55 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
-      <c r="C3" s="13"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
-      <c r="C4" s="13"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="13"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="13"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="13"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="13"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="13"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
@@ -1126,14 +1147,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AC15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
@@ -1152,9 +1174,7 @@
       <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="4"/>
@@ -1180,6 +1200,135 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="13"/>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="20"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>16.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>16.98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>16.98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>16.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>16.98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15">
+        <v>16.98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1190,7 +1339,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1201,13 +1350,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
partial working for incoming shipments
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7B3ACC-B30B-4741-8E48-D7CFFFF249AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC7AAB3-8E23-4F0A-B90D-D147A6905788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="1935" windowWidth="28800" windowHeight="15435" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26355" yWindow="2940" windowWidth="22605" windowHeight="9900" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="Hell" sheetId="11" r:id="rId4"/>
     <sheet name="Test" sheetId="10" r:id="rId5"/>
     <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId7"/>
+    <sheet name="incoming_shipment" sheetId="12" r:id="rId7"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -232,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -275,6 +276,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,15 +501,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -528,7 +532,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -545,7 +549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -562,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>1</v>
       </c>
@@ -579,7 +583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>2</v>
       </c>
@@ -596,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>2</v>
       </c>
@@ -613,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>2</v>
       </c>
@@ -630,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>3</v>
       </c>
@@ -647,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>3</v>
       </c>
@@ -664,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>3</v>
       </c>
@@ -681,12 +685,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
@@ -707,56 +711,56 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -768,17 +772,17 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E12" sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -795,7 +799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -812,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -829,7 +833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -846,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -863,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -880,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -897,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
@@ -914,7 +918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -931,7 +935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -948,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -965,7 +969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -982,7 +986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
     </row>
   </sheetData>
@@ -998,9 +1002,9 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1017,7 +1021,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1047,9 +1051,9 @@
       <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1066,7 +1070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1083,54 +1087,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="11"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="3"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="3"/>
       <c r="C6" s="11"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="3"/>
       <c r="C7" s="11"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="3"/>
       <c r="C8" s="11"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="3"/>
       <c r="C9" s="11"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="3"/>
       <c r="C10" s="11"/>
@@ -1149,19 +1153,19 @@
   </sheetPr>
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" customWidth="1"/>
     <col min="3" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1200,28 +1204,28 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -1231,7 +1235,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1245,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1259,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1273,7 +1277,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1287,7 +1291,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1301,7 +1305,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1315,7 +1319,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1329,7 +1333,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1343,7 +1347,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1363,6 +1367,157 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -1370,13 +1525,13 @@
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
working UpdateInventory (incoming shipment)
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC7AAB3-8E23-4F0A-B90D-D147A6905788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7961B23-B161-4E69-878B-0B00C1BA61C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26355" yWindow="2940" windowWidth="22605" windowHeight="9900" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1760" yWindow="740" windowWidth="13750" windowHeight="8690" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
     <sheet name="vendors" sheetId="2" r:id="rId2"/>
     <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
-    <sheet name="Hell" sheetId="11" r:id="rId4"/>
-    <sheet name="Test" sheetId="10" r:id="rId5"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
-    <sheet name="incoming_shipment" sheetId="12" r:id="rId7"/>
+    <sheet name="incoming_shipment" sheetId="12" r:id="rId4"/>
+    <sheet name="Hell" sheetId="11" r:id="rId5"/>
+    <sheet name="Test" sheetId="10" r:id="rId6"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId7"/>
     <sheet name="out_of_stock" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="A1:E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -782,38 +782,38 @@
     <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="2">
         <v>24.99</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="3">
-        <v>1</v>
+      <c r="E2" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -830,7 +830,7 @@
         <v>0.5</v>
       </c>
       <c r="E3" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -847,24 +847,24 @@
         <v>0.1</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="11">
         <v>2.99</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="3">
         <v>0.1</v>
       </c>
-      <c r="E5" s="2">
-        <v>2</v>
+      <c r="E5" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -874,14 +874,14 @@
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>1.99</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="10">
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -897,8 +897,8 @@
       <c r="D7" s="2">
         <v>0.5</v>
       </c>
-      <c r="E7" s="3">
-        <v>3</v>
+      <c r="E7" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -911,11 +911,11 @@
       <c r="C8" s="11">
         <v>1999</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.1</v>
       </c>
       <c r="E8" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>0.5</v>
       </c>
       <c r="E9" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -949,24 +949,24 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="11">
         <v>5.99</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>0</v>
       </c>
-      <c r="E11">
-        <v>3</v>
+      <c r="E11" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -995,6 +995,157 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBA6BF3-9357-4785-B233-4123450A0704}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1043,7 +1194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1146,7 +1297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1366,157 +1517,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>

</xml_diff>

<commit_message>
all orders now run
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7B3ACC-B30B-4741-8E48-D7CFFFF249AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA62C46-10E5-4C5F-8EA9-5BE183D5EC8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="1935" windowWidth="28800" windowHeight="15435" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5265" yWindow="1935" windowWidth="28800" windowHeight="15435" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
     <sheet name="vendors" sheetId="2" r:id="rId2"/>
     <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
-    <sheet name="Hell" sheetId="11" r:id="rId4"/>
-    <sheet name="Test" sheetId="10" r:id="rId5"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId7"/>
+    <sheet name="Walmart" sheetId="12" r:id="rId4"/>
+    <sheet name="Hell" sheetId="11" r:id="rId5"/>
+    <sheet name="Test" sheetId="10" r:id="rId6"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId7"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -148,10 +149,22 @@
     <t>Column2</t>
   </si>
   <si>
-    <t>Carson Goble</t>
-  </si>
-  <si>
-    <t>kcbku98@gmail.com</t>
+    <t>Walmart</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Cindy</t>
+  </si>
+  <si>
+    <t>Cayden Doyle</t>
+  </si>
+  <si>
+    <t>kenny.bradburn@revature.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -232,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -249,9 +262,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -272,9 +282,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,7 +501,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D7" sqref="D5:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -529,162 +536,174 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="A4" s="14">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="15">
+      <c r="A5" s="14">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
+      <c r="A6" s="14">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>2</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>3</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>3</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="12">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
@@ -701,7 +720,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
@@ -719,44 +738,49 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-    </row>
     <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="5"/>
     </row>
     <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="A15" s="7"/>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+    </row>
     <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -765,10 +789,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -982,8 +1006,30 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+    </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -991,11 +1037,63 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43194B3-AE81-4476-A0CE-22872FC6E9CC}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBA6BF3-9357-4785-B233-4123450A0704}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1039,7 +1137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1142,15 +1240,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1200,161 +1298,33 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="13"/>
-    </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="12"/>
-    </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>16.98</v>
-      </c>
-    </row>
+    <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
       </c>
       <c r="D14">
-        <v>16.98</v>
+        <v>1801.7909999999999</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17">
-        <v>9.4849999999999994</v>
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Tim's Update Inventory SG to Main
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7961B23-B161-4E69-878B-0B00C1BA61C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7767DEF3-6E6F-4E89-9E98-E4A02960904E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="740" windowWidth="13750" windowHeight="8690" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="3870" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>kcbku98@gmail.com</t>
+  </si>
+  <si>
+    <t>Cindy</t>
+  </si>
+  <si>
+    <t>Test Email</t>
   </si>
 </sst>
 </file>
@@ -498,18 +504,18 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -532,7 +538,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -549,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -566,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>1</v>
       </c>
@@ -583,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>2</v>
       </c>
@@ -600,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>2</v>
       </c>
@@ -617,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>2</v>
       </c>
@@ -634,7 +640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>3</v>
       </c>
@@ -651,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>3</v>
       </c>
@@ -668,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>3</v>
       </c>
@@ -685,12 +691,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="13">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
@@ -711,56 +729,56 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
     </row>
-    <row r="19" ht="12.5" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="12.5" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -775,14 +793,14 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -799,7 +817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
@@ -813,10 +831,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -830,10 +848,10 @@
         <v>0.5</v>
       </c>
       <c r="E3" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -847,10 +865,10 @@
         <v>0.1</v>
       </c>
       <c r="E4" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -864,10 +882,10 @@
         <v>0.1</v>
       </c>
       <c r="E5" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -881,10 +899,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -898,10 +916,10 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
@@ -915,10 +933,10 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -932,10 +950,10 @@
         <v>0.5</v>
       </c>
       <c r="E9" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -949,10 +967,10 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>33</v>
       </c>
@@ -969,7 +987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -983,10 +1001,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
     </row>
   </sheetData>
@@ -1002,13 +1020,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1019,7 +1037,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1030,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1041,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1052,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -1063,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -1074,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -1085,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
@@ -1096,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -1107,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -1118,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1129,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1153,9 +1171,9 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1172,7 +1190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1202,9 +1220,9 @@
       <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1221,7 +1239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1238,54 +1256,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" s="11"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="3"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="3"/>
       <c r="C6" s="11"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="3"/>
       <c r="C7" s="11"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="3"/>
       <c r="C8" s="11"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="3"/>
       <c r="C9" s="11"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="3"/>
       <c r="C10" s="11"/>
@@ -1302,21 +1320,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.54296875" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1355,24 +1373,24 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="13"/>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="20"/>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1386,7 +1404,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1400,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1414,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1428,7 +1446,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1442,7 +1460,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1456,7 +1474,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1470,7 +1488,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1484,7 +1502,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1498,7 +1516,7 @@
         <v>16.98</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1510,6 +1528,20 @@
       </c>
       <c r="D17">
         <v>9.4849999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>13.98</v>
       </c>
     </row>
   </sheetData>
@@ -1525,13 +1557,13 @@
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
notify discount groundwork and is partially working
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,33 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7767DEF3-6E6F-4E89-9E98-E4A02960904E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9DAA61-4745-4082-81EB-8613153178D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="3870" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1760" yWindow="740" windowWidth="16690" windowHeight="8690" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
     <sheet name="vendors" sheetId="2" r:id="rId2"/>
     <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
     <sheet name="incoming_shipment" sheetId="12" r:id="rId4"/>
-    <sheet name="Hell" sheetId="11" r:id="rId5"/>
-    <sheet name="Test" sheetId="10" r:id="rId6"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId7"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId8"/>
+    <sheet name="Test" sheetId="10" r:id="rId5"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -159,6 +158,12 @@
   </si>
   <si>
     <t>Test Email</t>
+  </si>
+  <si>
+    <t>Aiden Herrera</t>
+  </si>
+  <si>
+    <t>kcbradburn98@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -239,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -256,9 +261,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -279,12 +281,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,15 +503,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -538,161 +534,161 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="14" t="s">
+    <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14" t="s">
+    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="15">
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="15">
+      <c r="E6" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
         <v>2</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
+    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
         <v>3</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>3</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -704,11 +700,11 @@
       <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
@@ -729,56 +725,56 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -789,18 +785,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -817,7 +813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
@@ -831,10 +827,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -848,10 +844,10 @@
         <v>0.5</v>
       </c>
       <c r="E3" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -865,10 +861,10 @@
         <v>0.1</v>
       </c>
       <c r="E4" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -882,10 +878,10 @@
         <v>0.1</v>
       </c>
       <c r="E5" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -899,10 +895,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -916,10 +912,10 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
@@ -933,10 +929,10 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -950,10 +946,10 @@
         <v>0.5</v>
       </c>
       <c r="E9" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -967,10 +963,10 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>33</v>
       </c>
@@ -987,24 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12">
-        <v>6.99</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
     </row>
   </sheetData>
@@ -1017,16 +996,16 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1037,7 +1016,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1048,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1059,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1070,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -1081,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -1092,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -1103,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
@@ -1114,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -1125,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -1136,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1144,19 +1123,11 @@
         <v>33</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1164,16 +1135,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBA6BF3-9357-4785-B233-4123450A0704}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F11" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1190,15 +1161,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="11">
-        <v>6.99</v>
+        <v>5.99</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -1206,6 +1177,60 @@
       <c r="E2" s="3">
         <v>3</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1213,128 +1238,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="11">
-        <v>5.99</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC18"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="4" width="15" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1373,175 +1296,32 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="13"/>
-    </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="12"/>
-    </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="D15">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16">
-        <v>16.98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17">
-        <v>9.4849999999999994</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18">
-        <v>13.98</v>
+      <c r="D2">
+        <v>59.464999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <v>3009.1860000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1549,7 +1329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -1557,13 +1337,13 @@
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
email for discount is now dynamic with 17 second delay. emails are sent to one test email address
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9DAA61-4745-4082-81EB-8613153178D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E4AC53-C8EC-43BA-96C7-5A38C0991092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1760" yWindow="740" windowWidth="16690" windowHeight="8690" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20460" yWindow="4215" windowWidth="16695" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -46,18 +46,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t xml:space="preserve">
-kcbku98@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kcbradburn98@gmail.com
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kenny.bradburn@revature.net
-</t>
-  </si>
-  <si>
     <t>Order Number</t>
   </si>
   <si>
@@ -157,20 +145,20 @@
     <t>Cindy</t>
   </si>
   <si>
-    <t>Test Email</t>
-  </si>
-  <si>
     <t>Aiden Herrera</t>
   </si>
   <si>
     <t>kcbradburn98@gmail.com</t>
+  </si>
+  <si>
+    <t>testemail22113355@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -223,6 +211,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,10 +236,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -282,8 +278,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -499,9 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -512,9 +516,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="A1" s="20"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
@@ -522,16 +524,16 @@
         <v>4</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
@@ -541,17 +543,17 @@
       <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>5</v>
+      <c r="C2" s="21" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -559,10 +561,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3" s="14">
         <v>1</v>
@@ -576,10 +578,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E4" s="14">
         <v>1</v>
@@ -593,10 +595,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" s="14">
         <v>1</v>
@@ -610,10 +612,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="18">
         <v>1</v>
@@ -626,11 +628,11 @@
       <c r="B7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>6</v>
+      <c r="C7" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" s="12">
         <v>2</v>
@@ -644,10 +646,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E8" s="12">
         <v>1</v>
@@ -661,10 +663,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E9" s="16">
         <v>1</v>
@@ -678,27 +680,27 @@
         <v>3</v>
       </c>
       <c r="C10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>7</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>10</v>
       </c>
       <c r="E10" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" s="12">
         <v>2</v>
@@ -710,6 +712,9 @@
       <c r="D12" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A2D9E92F-C751-46F1-9FE3-BDED1F19E007}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -737,27 +742,27 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -786,7 +791,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -798,27 +803,27 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2">
         <v>24.99</v>
@@ -832,10 +837,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="11">
         <v>4.99</v>
@@ -849,10 +854,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" s="11">
         <v>12.99</v>
@@ -866,10 +871,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="11">
         <v>2.99</v>
@@ -883,10 +888,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="10">
         <v>1.99</v>
@@ -900,10 +905,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="11">
         <v>1</v>
@@ -917,10 +922,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="11">
         <v>1999</v>
@@ -934,10 +939,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" s="11">
         <v>2999</v>
@@ -951,10 +956,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11">
         <v>14.99</v>
@@ -968,10 +973,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="11">
         <v>5.99</v>
@@ -1007,21 +1012,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -1029,10 +1034,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1040,10 +1045,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1051,10 +1056,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -1062,10 +1067,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -1073,10 +1078,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1084,10 +1089,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -1095,10 +1100,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -1106,10 +1111,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -1117,10 +1122,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -1146,27 +1151,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="11">
         <v>5.99</v>
@@ -1244,7 +1249,7 @@
   </sheetPr>
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1259,7 +1264,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1268,7 +1273,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1301,10 +1306,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>59.464999999999996</v>
@@ -1315,10 +1320,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>3009.1860000000001</v>
@@ -1345,13 +1350,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
readme update and source sheet update
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E4AC53-C8EC-43BA-96C7-5A38C0991092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB884B48-4A84-488A-9099-F14590D9E008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20460" yWindow="4215" windowWidth="16695" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Hell</t>
   </si>
   <si>
-    <t>Souls</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>testemail22113355@gmail.com</t>
+  </si>
+  <si>
+    <t>Order No.</t>
   </si>
 </sst>
 </file>
@@ -240,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -280,9 +280,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -505,7 +502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -516,7 +515,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
+      <c r="A1" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
@@ -530,10 +531,10 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
@@ -543,8 +544,8 @@
       <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>40</v>
+      <c r="C2" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>7</v>
@@ -561,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>10</v>
@@ -578,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -595,7 +596,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>8</v>
@@ -612,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>10</v>
@@ -629,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>12</v>
@@ -646,7 +647,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>9</v>
@@ -663,7 +664,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>8</v>
@@ -680,7 +681,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>7</v>
@@ -694,13 +695,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E11" s="12">
         <v>2</v>
@@ -1306,10 +1307,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
       </c>
       <c r="D2">
         <v>59.464999999999996</v>
@@ -1320,10 +1321,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
       </c>
       <c r="D3">
         <v>3009.1860000000001</v>

</xml_diff>

<commit_message>
bugfix for sheet name in client list making runorder not work
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB884B48-4A84-488A-9099-F14590D9E008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B398A14-79F2-4A1B-9E53-B426CF698793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20460" yWindow="4215" windowWidth="16695" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-23025" yWindow="4290" windowWidth="21555" windowHeight="11235" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>testemail22113355@gmail.com</t>
-  </si>
-  <si>
-    <t>Order No.</t>
   </si>
 </sst>
 </file>
@@ -502,12 +499,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.81640625" customWidth="1"/>
@@ -516,7 +514,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -554,7 +552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -1248,9 +1246,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1330,6 +1328,20 @@
         <v>3009.1860000000001</v>
       </c>
     </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>3.98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated datatable output to sheet1 missing email
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B398A14-79F2-4A1B-9E53-B426CF698793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7747058D-480D-46E4-8393-2CF8767071E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-23025" yWindow="4290" windowWidth="21555" windowHeight="11235" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23100" yWindow="1920" windowWidth="21555" windowHeight="11055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
-    <sheet name="vendors" sheetId="2" r:id="rId2"/>
-    <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
-    <sheet name="incoming_shipment" sheetId="12" r:id="rId4"/>
-    <sheet name="Test" sheetId="10" r:id="rId5"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
+    <sheet name="vendors" sheetId="2" r:id="rId3"/>
+    <sheet name="vendor_inventory" sheetId="8" r:id="rId4"/>
+    <sheet name="incoming_shipment" sheetId="12" r:id="rId5"/>
+    <sheet name="Test" sheetId="10" r:id="rId6"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId7"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -237,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -280,6 +281,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -719,6 +723,122 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC3B394-B843-4C1B-BE8B-87A5699CA40F}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>59.465000000000003</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="50" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1876.761</v>
+      </c>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" ht="50" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3009.1860000000001</v>
+      </c>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>3.98</v>
+      </c>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="D18" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -785,7 +905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -995,7 +1115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1138,7 +1258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1241,14 +1361,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1347,7 +1467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>
   <sheetViews>

</xml_diff>

<commit_message>
experimental loop update for formmating output to sheet1
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED1CBD8-7B50-4545-9587-20D7E7AE73FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA50EC09-ADE4-4D5A-924B-F0E66786508F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23100" yWindow="2490" windowWidth="21555" windowHeight="10485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -724,10 +724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC3B394-B843-4C1B-BE8B-87A5699CA40F}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D4" sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -736,107 +736,132 @@
     <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="21">
+      <c r="D2" s="21">
         <v>59.465000000000003</v>
       </c>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" ht="50" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="21">
+      <c r="D3" s="21">
         <v>3009.1860000000001</v>
       </c>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:4" ht="50" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="21">
+      <c r="D4" s="21">
         <v>1876.761</v>
       </c>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>39</v>
       </c>
-      <c r="C5">
+      <c r="D5" s="21">
         <v>3.98</v>
       </c>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
       <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
       <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
       <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="D12" s="21"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="D13" s="21"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="D14" s="21"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="D15" s="21"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="D16" s="21"/>
     </row>

</xml_diff>

<commit_message>
have two datatables that aren't joining
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA50EC09-ADE4-4D5A-924B-F0E66786508F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E890C477-324B-42C3-9402-89E3CBD61AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23100" yWindow="2490" windowWidth="21555" windowHeight="10485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27510" yWindow="3525" windowWidth="17820" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -727,7 +727,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:E11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -736,79 +736,36 @@
     <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>20</v>
-      </c>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="21">
-        <v>59.465000000000003</v>
-      </c>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="21">
-        <v>3009.1860000000001</v>
-      </c>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="21">
-        <v>1876.761</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="21">
-        <v>3.98</v>
-      </c>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
works with temp sheets sheet1/sheet2
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E890C477-324B-42C3-9402-89E3CBD61AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C5A5C0-D4A0-4AEF-8F39-8B63D458D62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27510" yWindow="3525" windowWidth="17820" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="450" windowWidth="16510" windowHeight="9150" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="clients" sheetId="7" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
-    <sheet name="vendors" sheetId="2" r:id="rId3"/>
-    <sheet name="vendor_inventory" sheetId="8" r:id="rId4"/>
-    <sheet name="incoming_shipment" sheetId="12" r:id="rId5"/>
-    <sheet name="Test" sheetId="10" r:id="rId6"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId7"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId2"/>
+    <sheet name="clients" sheetId="7" r:id="rId3"/>
+    <sheet name="vendors" sheetId="2" r:id="rId4"/>
+    <sheet name="vendor_inventory" sheetId="8" r:id="rId5"/>
+    <sheet name="incoming_shipment" sheetId="12" r:id="rId6"/>
+    <sheet name="Test" sheetId="10" r:id="rId7"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId8"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -134,19 +135,7 @@
     <t>Column2</t>
   </si>
   <si>
-    <t>Carson Goble</t>
-  </si>
-  <si>
-    <t>kcbku98@gmail.com</t>
-  </si>
-  <si>
     <t>Cindy</t>
-  </si>
-  <si>
-    <t>Aiden Herrera</t>
-  </si>
-  <si>
-    <t>kcbradburn98@gmail.com</t>
   </si>
   <si>
     <t>testemail22113355@gmail.com</t>
@@ -500,6 +489,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2B6E0B-2DB5-4EAB-8FF6-F9DE91881291}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9CDE765-175A-421A-8844-7A3E936E2E86}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>59.465000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1876.761</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3009.1860000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -547,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>7</v>
@@ -564,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>10</v>
@@ -581,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -598,7 +708,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>8</v>
@@ -615,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>10</v>
@@ -632,7 +742,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>12</v>
@@ -649,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>9</v>
@@ -666,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>8</v>
@@ -683,7 +793,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>7</v>
@@ -697,10 +807,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>11</v>
@@ -722,120 +832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC3B394-B843-4C1B-BE8B-87A5699CA40F}">
-  <dimension ref="A1:E18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="23.08984375" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="D18" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -902,7 +899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -1112,7 +1109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1255,7 +1252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1358,15 +1355,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1421,25 +1418,25 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
+      <c r="B2" s="21" t="s">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
       </c>
       <c r="D2">
-        <v>59.464999999999996</v>
+        <v>59.465000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>37</v>
+      <c r="B3" s="21" t="s">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>3009.1860000000001</v>
@@ -1447,15 +1444,29 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>1876.761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
         <v>3.98</v>
       </c>
     </row>
@@ -1464,7 +1475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>
   <sheetViews>

</xml_diff>

<commit_message>
runorderall working and added to main.xaml. calc1/2 sheets in source required for it to work properly
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,27 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C5A5C0-D4A0-4AEF-8F39-8B63D458D62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E023C0-0DBE-4E4B-B472-51557D2B2C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="450" windowWidth="16510" windowHeight="9150" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22845" yWindow="3045" windowWidth="20145" windowHeight="11280" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="17" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="16" r:id="rId2"/>
-    <sheet name="clients" sheetId="7" r:id="rId3"/>
-    <sheet name="vendors" sheetId="2" r:id="rId4"/>
-    <sheet name="vendor_inventory" sheetId="8" r:id="rId5"/>
-    <sheet name="incoming_shipment" sheetId="12" r:id="rId6"/>
-    <sheet name="Test" sheetId="10" r:id="rId7"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId8"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId9"/>
+    <sheet name="clients" sheetId="7" r:id="rId1"/>
+    <sheet name="vendors" sheetId="2" r:id="rId2"/>
+    <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
+    <sheet name="incoming_shipment" sheetId="12" r:id="rId4"/>
+    <sheet name="Test" sheetId="10" r:id="rId5"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId7"/>
+    <sheet name="calc2" sheetId="19" r:id="rId8"/>
+    <sheet name="calc1" sheetId="18" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>testemail22113355@gmail.com</t>
+  </si>
+  <si>
+    <t>Carson Goble</t>
+  </si>
+  <si>
+    <t>Aiden Herrera</t>
+  </si>
+  <si>
+    <t>Cayden Doyle</t>
   </si>
 </sst>
 </file>
@@ -489,127 +498,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2B6E0B-2DB5-4EAB-8FF6-F9DE91881291}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="50" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="50" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9CDE765-175A-421A-8844-7A3E936E2E86}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>59.465000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1876.761</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3009.1860000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>3.98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -832,7 +720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -899,7 +787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -1109,7 +997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1252,7 +1140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1355,7 +1243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1419,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
@@ -1433,7 +1321,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -1447,7 +1335,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1475,7 +1363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -1503,4 +1391,125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2735A956-B3D6-4E65-A566-E302C3A3474A}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513E0CE4-7397-430C-962C-BB4312245C77}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>59.465000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1876.761</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3009.1860000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
inventory management is now working 100%
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E023C0-0DBE-4E4B-B472-51557D2B2C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C6F4F5-4E24-4C9F-94DF-804157A213CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22845" yWindow="3045" windowWidth="20145" windowHeight="11280" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10200" yWindow="2970" windowWidth="23475" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -96,12 +96,6 @@
     <t>Total Expenses</t>
   </si>
   <si>
-    <t>Items Out of Stock</t>
-  </si>
-  <si>
-    <t>Items Not Found</t>
-  </si>
-  <si>
     <t>Order</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Hell</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -141,13 +132,7 @@
     <t>testemail22113355@gmail.com</t>
   </si>
   <si>
-    <t>Carson Goble</t>
-  </si>
-  <si>
-    <t>Aiden Herrera</t>
-  </si>
-  <si>
-    <t>Cayden Doyle</t>
+    <t>Client Name</t>
   </si>
 </sst>
 </file>
@@ -501,20 +486,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -525,36 +509,36 @@
         <v>4</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>35</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -562,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>10</v>
@@ -571,7 +555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>1</v>
       </c>
@@ -579,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -588,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
         <v>2</v>
       </c>
@@ -596,7 +580,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>8</v>
@@ -605,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>2</v>
       </c>
@@ -613,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>10</v>
@@ -622,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>2</v>
       </c>
@@ -630,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>12</v>
@@ -639,7 +623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
         <v>3</v>
       </c>
@@ -647,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>9</v>
@@ -656,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>3</v>
       </c>
@@ -664,7 +648,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>8</v>
@@ -673,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>3</v>
       </c>
@@ -681,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>7</v>
@@ -690,15 +674,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>11</v>
@@ -707,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
@@ -728,59 +712,54 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-    </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-    </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="19" ht="12.5" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="12.5" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -792,19 +771,19 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>13</v>
@@ -819,43 +798,43 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="8">
         <v>24.99</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="8">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="E2" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="2">
         <v>4.99</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
@@ -870,9 +849,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -887,43 +866,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>27</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="11">
         <v>1.99</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10">
         <v>0.5</v>
       </c>
       <c r="E7" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -934,13 +913,13 @@
       <c r="D8" s="2">
         <v>0.1</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -948,16 +927,16 @@
       <c r="C9" s="11">
         <v>2999</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.5</v>
       </c>
       <c r="E9" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
@@ -969,15 +948,15 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="11">
         <v>5.99</v>
@@ -989,7 +968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
     </row>
   </sheetData>
@@ -1005,15 +984,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -1022,9 +1001,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -1033,9 +1012,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
@@ -1044,9 +1023,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
@@ -1055,9 +1034,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -1066,9 +1045,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -1077,9 +1056,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
@@ -1088,9 +1067,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -1099,9 +1078,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -1110,9 +1089,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
@@ -1121,18 +1100,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C12" s="3"/>
     </row>
   </sheetData>
@@ -1148,11 +1127,11 @@
       <selection activeCell="F11" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -1167,12 +1146,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="11">
         <v>5.99</v>
@@ -1184,54 +1163,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" s="11"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="3"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="3"/>
       <c r="C6" s="11"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="3"/>
       <c r="C7" s="11"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="3"/>
       <c r="C8" s="11"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="3"/>
       <c r="C9" s="11"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="3"/>
       <c r="C10" s="11"/>
@@ -1248,22 +1227,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1302,62 +1281,6 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2">
-        <v>59.465000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>3009.1860000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4">
-        <v>1876.761</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5">
-        <v>3.98</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1365,31 +1288,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1399,9 +1327,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1412,7 +1340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1420,10 +1348,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1431,10 +1359,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1442,18 +1370,18 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1467,9 +1395,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1477,7 +1405,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1485,7 +1413,7 @@
         <v>59.465000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1493,7 +1421,7 @@
         <v>1876.761</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1501,7 +1429,7 @@
         <v>3009.1860000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Code is now working with add client modularly, emails work, inventory additions work, order picking numbers work, out of stock works.
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -8,27 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C6F4F5-4E24-4C9F-94DF-804157A213CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7255A09F-C337-4CC5-972A-0694672BF5D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="2970" windowWidth="23475" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10200" yWindow="2970" windowWidth="27000" windowHeight="15915" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
-    <sheet name="vendors" sheetId="2" r:id="rId2"/>
-    <sheet name="vendor_inventory" sheetId="8" r:id="rId3"/>
-    <sheet name="incoming_shipment" sheetId="12" r:id="rId4"/>
-    <sheet name="Test" sheetId="10" r:id="rId5"/>
-    <sheet name="expense_reports" sheetId="6" r:id="rId6"/>
-    <sheet name="out_of_stock" sheetId="9" r:id="rId7"/>
-    <sheet name="calc2" sheetId="19" r:id="rId8"/>
-    <sheet name="calc1" sheetId="18" r:id="rId9"/>
+    <sheet name="Michel" sheetId="20" r:id="rId2"/>
+    <sheet name="Tammy" sheetId="21" r:id="rId3"/>
+    <sheet name="vendors" sheetId="2" r:id="rId4"/>
+    <sheet name="vendor_inventory" sheetId="8" r:id="rId5"/>
+    <sheet name="incoming_shipment" sheetId="12" r:id="rId6"/>
+    <sheet name="Test" sheetId="10" r:id="rId7"/>
+    <sheet name="expense_reports" sheetId="6" r:id="rId8"/>
+    <sheet name="out_of_stock" sheetId="9" r:id="rId9"/>
+    <sheet name="calc2" sheetId="19" r:id="rId10"/>
+    <sheet name="calc1" sheetId="18" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -120,12 +122,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t>Cindy</t>
   </si>
   <si>
@@ -133,6 +129,24 @@
   </si>
   <si>
     <t>Client Name</t>
+  </si>
+  <si>
+    <t>Michel</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>Carson Goble</t>
+  </si>
+  <si>
+    <t>Aiden Herrera</t>
+  </si>
+  <si>
+    <t>Cayden Doyle</t>
   </si>
 </sst>
 </file>
@@ -221,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -238,26 +252,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -267,6 +269,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -484,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="A12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -514,187 +519,212 @@
       <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1"/>
+      <c r="G1"/>
+    </row>
+    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>2</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>2</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>3</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>3</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>3</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>4</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="14">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="C11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
-        <v>1</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
-        <v>2</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
-        <v>2</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="14">
-        <v>2</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="14">
-        <v>3</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="14">
-        <v>3</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
-        <v>3</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
-        <v>4</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="3"/>
+      <c r="E13">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -704,7 +734,254 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2735A956-B3D6-4E65-A566-E302C3A3474A}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513E0CE4-7397-430C-962C-BB4312245C77}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>84.454999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1876.761</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>134.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3009.1860000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7100FFB1-2534-4A44-8173-6833FA3E030E}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EFB47B-9BBD-4476-997A-4D5651B7181C}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -766,12 +1043,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -812,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -829,7 +1106,7 @@
         <v>0.5</v>
       </c>
       <c r="E3" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -846,7 +1123,7 @@
         <v>0.1</v>
       </c>
       <c r="E4" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -863,7 +1140,7 @@
         <v>0.1</v>
       </c>
       <c r="E5" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -897,7 +1174,7 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -914,7 +1191,7 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -931,7 +1208,7 @@
         <v>0.5</v>
       </c>
       <c r="E9" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -948,7 +1225,7 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -965,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -976,7 +1253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1119,7 +1396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1222,14 +1499,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1281,14 +1558,84 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>84.454999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>3009.1860000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>1876.761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>134.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -1309,135 +1656,42 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2735A956-B3D6-4E65-A566-E302C3A3474A}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513E0CE4-7397-430C-962C-BB4312245C77}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>59.465000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1876.761</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3009.1860000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>3.98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated with initial version of powerpoint
</commit_message>
<xml_diff>
--- a/P0 source datasheet.xlsx
+++ b/P0 source datasheet.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Yu_Timothy_Bradburn_Kenneth_P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_Timothy_Bradburn_Kenneth_P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7255A09F-C337-4CC5-972A-0694672BF5D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712268E3-F716-4A28-8E6F-33B1AE7174CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="2970" windowWidth="27000" windowHeight="15915" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="170" yWindow="730" windowWidth="16350" windowHeight="9220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
     <sheet name="Michel" sheetId="20" r:id="rId2"/>
     <sheet name="Tammy" sheetId="21" r:id="rId3"/>
-    <sheet name="vendors" sheetId="2" r:id="rId4"/>
-    <sheet name="vendor_inventory" sheetId="8" r:id="rId5"/>
-    <sheet name="incoming_shipment" sheetId="12" r:id="rId6"/>
-    <sheet name="Test" sheetId="10" r:id="rId7"/>
+    <sheet name="Test" sheetId="10" r:id="rId4"/>
+    <sheet name="vendors" sheetId="2" r:id="rId5"/>
+    <sheet name="vendor_inventory" sheetId="8" r:id="rId6"/>
+    <sheet name="incoming_shipment" sheetId="12" r:id="rId7"/>
     <sheet name="expense_reports" sheetId="6" r:id="rId8"/>
     <sheet name="out_of_stock" sheetId="9" r:id="rId9"/>
     <sheet name="calc2" sheetId="19" r:id="rId10"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -273,6 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -491,19 +492,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A12:E13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -522,7 +523,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -539,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -556,7 +557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -573,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -590,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -607,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -624,7 +625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -641,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>3</v>
       </c>
@@ -658,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>3</v>
       </c>
@@ -675,14 +676,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>4</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -692,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -700,7 +701,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -709,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -717,7 +718,7 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -729,6 +730,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A2D9E92F-C751-46F1-9FE3-BDED1F19E007}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{A25CCCFC-7C19-4AD1-B130-2CFC5DB923F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -740,9 +742,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -753,7 +755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -764,7 +766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -775,7 +777,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -786,7 +788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -797,7 +799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -817,11 +819,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513E0CE4-7397-430C-962C-BB4312245C77}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -829,7 +833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -837,7 +841,7 @@
         <v>84.454999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -845,7 +849,7 @@
         <v>1876.761</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -853,7 +857,7 @@
         <v>134.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -861,7 +865,7 @@
         <v>3009.1860000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -882,16 +886,16 @@
       <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -905,7 +909,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
@@ -932,9 +936,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -948,7 +952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
@@ -962,7 +966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>34</v>
       </c>
@@ -982,6 +986,109 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F10:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="11">
+        <v>5.99</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -992,73 +1099,73 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B886C4E3-F2D1-4830-A193-EEF23A4B9EC3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E10" sqref="D8:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>27</v>
       </c>
@@ -1075,7 +1182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>22</v>
       </c>
@@ -1089,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -1106,10 +1213,10 @@
         <v>0.5</v>
       </c>
       <c r="E3" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1123,10 +1230,10 @@
         <v>0.1</v>
       </c>
       <c r="E4" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1140,10 +1247,10 @@
         <v>0.1</v>
       </c>
       <c r="E5" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1157,10 +1264,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -1174,10 +1281,10 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
@@ -1191,10 +1298,10 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
@@ -1208,10 +1315,10 @@
         <v>0.5</v>
       </c>
       <c r="E9" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
@@ -1225,10 +1332,10 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
@@ -1242,154 +1349,11 @@
         <v>0</v>
       </c>
       <c r="E11" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1397,16 +1361,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7F312-233A-4C66-A68B-ECE14CEA95C6}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D158008C-85FB-44F2-B4DB-02DE0837DDBA}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F10:F11"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>27</v>
       </c>
@@ -1414,85 +1382,121 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="11">
-        <v>5.99</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1504,22 +1508,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1558,7 +1562,7 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1572,7 +1576,7 @@
         <v>84.454999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1586,7 +1590,7 @@
         <v>3009.1860000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1600,7 +1604,7 @@
         <v>1876.761</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1614,41 +1618,58 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
+      <c r="C6" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="D6">
         <v>134.9</v>
       </c>
     </row>
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>9.4849999999999994</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{9B74F6B5-0D46-4DEF-863C-680230ACC6D5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2604B47-8BEC-4F97-9F72-6906BB82C7E8}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>27</v>
       </c>
@@ -1662,7 +1683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1674,20 +1695,6 @@
       </c>
       <c r="D2">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>